<commit_message>
Acceptance test + tweaks to product controller and routes
</commit_message>
<xml_diff>
--- a/P5-acceptance_test_plan.xlsx
+++ b/P5-acceptance_test_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiegoJ\Documents\OC Projects\Project 5\Project-5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9340FC14-9404-47EE-9A55-00D5FBBE6654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE054AF-DE86-4D26-8C5D-7E71EA7D286B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -655,16 +655,16 @@
   </sheetPr>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="7.27734375" customWidth="1"/>
     <col min="2" max="3" width="58.44140625" customWidth="1"/>
-    <col min="4" max="4" width="57.83203125" customWidth="1"/>
-    <col min="5" max="5" width="52.71875" customWidth="1"/>
+    <col min="4" max="4" width="57.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27.3" x14ac:dyDescent="0.4">
@@ -801,98 +801,98 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:5" ht="21.3" x14ac:dyDescent="0.95">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:5" ht="21.3" x14ac:dyDescent="0.95">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="11" spans="1:5" ht="21.3" x14ac:dyDescent="0.95">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="12" spans="1:5" ht="21.3" x14ac:dyDescent="0.95">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" spans="1:5" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="13" spans="1:5" ht="21.3" x14ac:dyDescent="0.95">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" spans="1:5" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:5" ht="21.3" x14ac:dyDescent="0.95">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
     </row>
-    <row r="15" spans="1:5" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="15" spans="1:5" ht="21.3" x14ac:dyDescent="0.95">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:5" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="16" spans="1:5" ht="21.3" x14ac:dyDescent="0.95">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" spans="1:5" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="17" spans="1:5" ht="21.3" x14ac:dyDescent="0.95">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="9"/>
     </row>
-    <row r="18" spans="1:5" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="18" spans="1:5" ht="21.3" x14ac:dyDescent="0.95">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="19" spans="1:5" ht="21.3" x14ac:dyDescent="0.95">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:5" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="20" spans="1:5" ht="21.3" x14ac:dyDescent="0.95">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
     </row>
-    <row r="21" spans="1:5" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="21" spans="1:5" ht="21.3" x14ac:dyDescent="0.95">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
     </row>
-    <row r="22" spans="1:5" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="22" spans="1:5" ht="21.3" x14ac:dyDescent="0.95">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>

</xml_diff>